<commit_message>
base shear to sa
</commit_message>
<xml_diff>
--- a/20180126_SmartCut/Meeting/20190301 Meeting/ida/20190221 base shear to sa.xlsx
+++ b/20180126_SmartCut/Meeting/20190301 Meeting/ida/20190221 base shear to sa.xlsx
@@ -379,8 +379,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="J36" sqref="J36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -1232,6 +1232,14 @@
         <f t="shared" ref="G23:G37" si="0">D6/299.5941/0.81</f>
         <v>0.31355675257429882</v>
       </c>
+      <c r="I23">
+        <f>D6/D23</f>
+        <v>238.65085513378227</v>
+      </c>
+      <c r="J23">
+        <f>299.5941*0.81</f>
+        <v>242.67122100000003</v>
+      </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
@@ -1248,6 +1256,14 @@
         <f t="shared" si="0"/>
         <v>0.45935360419190369</v>
       </c>
+      <c r="I24">
+        <f t="shared" ref="I24:I37" si="1">D7/D24</f>
+        <v>233.14774417140575</v>
+      </c>
+      <c r="J24">
+        <f t="shared" ref="J24:J37" si="2">299.5941*0.81</f>
+        <v>242.67122100000003</v>
+      </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
@@ -1264,6 +1280,14 @@
         <f t="shared" si="0"/>
         <v>0.52199926912635419</v>
       </c>
+      <c r="I25">
+        <f t="shared" si="1"/>
+        <v>245.04054535043875</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="2"/>
+        <v>242.67122100000003</v>
+      </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
@@ -1280,6 +1304,14 @@
         <f t="shared" si="0"/>
         <v>0.54655059406488082</v>
       </c>
+      <c r="I26">
+        <f t="shared" si="1"/>
+        <v>247.09022012906686</v>
+      </c>
+      <c r="J26">
+        <f t="shared" si="2"/>
+        <v>242.67122100000003</v>
+      </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
@@ -1296,6 +1328,14 @@
         <f t="shared" si="0"/>
         <v>0.56164467891312075</v>
       </c>
+      <c r="I27">
+        <f t="shared" si="1"/>
+        <v>249.14632719615096</v>
+      </c>
+      <c r="J27">
+        <f t="shared" si="2"/>
+        <v>242.67122100000003</v>
+      </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
@@ -1312,6 +1352,14 @@
         <f t="shared" si="0"/>
         <v>0.56816502357319076</v>
       </c>
+      <c r="I28">
+        <f t="shared" si="1"/>
+        <v>249.63209866708186</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="2"/>
+        <v>242.67122100000003</v>
+      </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
@@ -1328,6 +1376,14 @@
         <f t="shared" si="0"/>
         <v>0.57405447348039662</v>
       </c>
+      <c r="I29">
+        <f t="shared" si="1"/>
+        <v>249.97846660709092</v>
+      </c>
+      <c r="J29">
+        <f t="shared" si="2"/>
+        <v>242.67122100000003</v>
+      </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
@@ -1344,6 +1400,14 @@
         <f t="shared" si="0"/>
         <v>0.58026617008697523</v>
       </c>
+      <c r="I30">
+        <f t="shared" si="1"/>
+        <v>250.20238095238093</v>
+      </c>
+      <c r="J30">
+        <f t="shared" si="2"/>
+        <v>242.67122100000003</v>
+      </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
@@ -1360,6 +1424,14 @@
         <f t="shared" si="0"/>
         <v>0.58632127622582808</v>
       </c>
+      <c r="I31">
+        <f t="shared" si="1"/>
+        <v>250.3731402377328</v>
+      </c>
+      <c r="J31">
+        <f t="shared" si="2"/>
+        <v>242.67122100000003</v>
+      </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
@@ -1376,8 +1448,16 @@
         <f t="shared" si="0"/>
         <v>0.59245138095711813</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I32">
+        <f t="shared" si="1"/>
+        <v>250.50075444214841</v>
+      </c>
+      <c r="J32">
+        <f t="shared" si="2"/>
+        <v>242.67122100000003</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
       <c r="C33" s="1">
         <v>101.95699999999999</v>
@@ -1392,8 +1472,16 @@
         <f t="shared" si="0"/>
         <v>0.59386234348736389</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I33">
+        <f t="shared" si="1"/>
+        <v>250.52072559125955</v>
+      </c>
+      <c r="J33">
+        <f t="shared" si="2"/>
+        <v>242.67122100000003</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
       <c r="C34" s="1">
         <v>102.173</v>
@@ -1408,8 +1496,16 @@
         <f t="shared" si="0"/>
         <v>0.35259928906032079</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I34">
+        <f t="shared" si="1"/>
+        <v>254.74777006347429</v>
+      </c>
+      <c r="J34">
+        <f t="shared" si="2"/>
+        <v>242.67122100000003</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
       <c r="C35" s="1">
         <v>109.015</v>
@@ -1424,8 +1520,16 @@
         <f t="shared" si="0"/>
         <v>0.40552315843006365</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I35">
+        <f t="shared" si="1"/>
+        <v>256.1388439905154</v>
+      </c>
+      <c r="J35">
+        <f t="shared" si="2"/>
+        <v>242.67122100000003</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
       <c r="C36" s="1">
         <v>112.643</v>
@@ -1440,8 +1544,16 @@
         <f t="shared" si="0"/>
         <v>0.41867799395957211</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I36">
+        <f t="shared" si="1"/>
+        <v>256.48876737780944</v>
+      </c>
+      <c r="J36">
+        <f t="shared" si="2"/>
+        <v>242.67122100000003</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
       <c r="C37" s="1">
         <v>116.50700000000001</v>
@@ -1456,8 +1568,16 @@
         <f t="shared" si="0"/>
         <v>0.4200543417548469</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I37">
+        <f t="shared" si="1"/>
+        <v>256.34892692421829</v>
+      </c>
+      <c r="J37">
+        <f t="shared" si="2"/>
+        <v>242.67122100000003</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B39" s="2"/>
       <c r="C39" s="1">
         <v>0</v>
@@ -1469,7 +1589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B40" s="2"/>
       <c r="C40" s="1">
         <v>9.1039999999999992</v>
@@ -1481,7 +1601,7 @@
         <v>0.33900000000000002</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B41" s="2"/>
       <c r="C41" s="1">
         <v>17.942</v>
@@ -1493,7 +1613,7 @@
         <v>0.38900000000000001</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B42" s="2"/>
       <c r="C42" s="1">
         <v>29.530999999999999</v>
@@ -1505,7 +1625,7 @@
         <v>0.48</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B43" s="2"/>
       <c r="C43" s="1">
         <v>34.262</v>
@@ -1517,7 +1637,7 @@
         <v>0.50700000000000001</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B44" s="2"/>
       <c r="C44" s="1">
         <v>41.704000000000001</v>
@@ -1529,7 +1649,7 @@
         <v>0.55400000000000005</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B45" s="2"/>
       <c r="C45" s="1">
         <v>53.338000000000001</v>
@@ -1541,7 +1661,7 @@
         <v>0.624</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B46" s="2"/>
       <c r="C46" s="1">
         <v>64.963999999999999</v>
@@ -1553,7 +1673,7 @@
         <v>0.68500000000000005</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B47" s="2"/>
       <c r="C47" s="1">
         <v>76.594999999999999</v>
@@ -1565,7 +1685,7 @@
         <v>0.74</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B48" s="2"/>
       <c r="C48" s="1">
         <v>88.222999999999999</v>

</xml_diff>